<commit_message>
Local build ferdig kap 7
</commit_message>
<xml_diff>
--- a/u_diagram.xlsx
+++ b/u_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uinnlandet-my.sharepoint.com/personal/nils_kvilvang_inn_no/Documents/Undervisning/SPC_book/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{759BD21B-2434-49D4-8436-60460F049427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{759BD21B-2434-49D4-8436-60460F049427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B8795E00-D7FC-4FA2-8E93-850135170A17}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E5A421C-DD09-40A2-877B-6098F62DE878}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8E5A421C-DD09-40A2-877B-6098F62DE878}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +96,10 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Geneva"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,9 +119,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -140,8 +145,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{622EECF0-C4E3-4851-86CF-B62DFDD147E3}"/>
     <cellStyle name="Normal_Bpchart3" xfId="1" xr:uid="{342B1579-2E89-49DF-A0DC-9002D6AEDA43}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,15 +463,15 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,7 +482,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -487,7 +493,7 @@
         <v>4658</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -498,7 +504,7 @@
         <v>4909</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -509,7 +515,7 @@
         <v>4886</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -520,7 +526,7 @@
         <v>4970</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -531,7 +537,7 @@
         <v>4780</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -542,7 +548,7 @@
         <v>4973</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -553,7 +559,7 @@
         <v>5762</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -564,7 +570,7 @@
         <v>5441</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -575,7 +581,7 @@
         <v>5893</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
@@ -586,7 +592,7 @@
         <v>5743</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
@@ -597,7 +603,7 @@
         <v>4747</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -608,7 +614,7 @@
         <v>5118</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -619,7 +625,7 @@
         <v>5609</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3">
       <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
@@ -630,7 +636,7 @@
         <v>5722</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3">
       <c r="A16" s="4" t="s">
         <v>3</v>
       </c>
@@ -641,7 +647,7 @@
         <v>5261</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -652,7 +658,7 @@
         <v>6071</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
@@ -663,7 +669,7 @@
         <v>6072</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -674,7 +680,7 @@
         <v>5335</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
@@ -685,7 +691,7 @@
         <v>6483</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="4" t="s">
         <v>8</v>
       </c>
@@ -696,7 +702,7 @@
         <v>5752</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="6" t="s">
         <v>9</v>
       </c>
@@ -707,7 +713,7 @@
         <v>5731</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
@@ -718,7 +724,7 @@
         <v>5017</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
         <v>11</v>
       </c>
@@ -729,7 +735,7 @@
         <v>5158</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
         <v>12</v>
       </c>

</xml_diff>